<commit_message>
Included planning stage in docs. Now try to do front end
</commit_message>
<xml_diff>
--- a/docs/manual_tests.xlsx
+++ b/docs/manual_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Coder_Academy\Term_4_Assignment_real\ccc-03-16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA835B-975D-45DB-B5B1-8936758F9236}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C4AE954-A5E3-4487-9D39-AB793FA23B82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{F9969861-9E08-43B7-8AB0-936C696BF090}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9969861-9E08-43B7-8AB0-936C696BF090}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
   <si>
     <t>Feature</t>
   </si>
@@ -145,6 +145,129 @@
   </si>
   <si>
     <t>I forgot to change the expense field to the income field in the json</t>
+  </si>
+  <si>
+    <t>CRUD goals</t>
+  </si>
+  <si>
+    <t>Try to create, read, update and delete a goal</t>
+  </si>
+  <si>
+    <t>Error: create is missing data for required field</t>
+  </si>
+  <si>
+    <t>Can do CRUD operations on goals with ease</t>
+  </si>
+  <si>
+    <t>No default created_at time. This is causing the error.</t>
+  </si>
+  <si>
+    <t>Error: null value in column "goal_type" violates not-null constraint</t>
+  </si>
+  <si>
+    <t>Goal type is missing</t>
+  </si>
+  <si>
+    <t>AttributeError: type object 'Goal' has no attribute 'week_start'</t>
+  </si>
+  <si>
+    <t>I need to change week_start to created</t>
+  </si>
+  <si>
+    <t>CRUD exercise log item</t>
+  </si>
+  <si>
+    <t>Try to create, read, update and delete exercise log items</t>
+  </si>
+  <si>
+    <t>Error: exercise log item has no property 'username'</t>
+  </si>
+  <si>
+    <t>Can do CRUD operations on exercise log item</t>
+  </si>
+  <si>
+    <t>invalid input syntax for type integer: "test2@gmail.com"</t>
+  </si>
+  <si>
+    <t>AttributeError: type object 'ExerciseLogItem' has no attribute 'created'</t>
+  </si>
+  <si>
+    <t>(psycopg2.errors.NotNullViolation) null value in column "user_id" violates not-null constraint</t>
+  </si>
+  <si>
+    <t>Can upload, view and delete images</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Try to upload new images, see them in app and delete them</t>
+  </si>
+  <si>
+    <t>have not set user_id field</t>
+  </si>
+  <si>
+    <t>TypeError: user_image_show() got an unexpected keyword argument 'id'</t>
+  </si>
+  <si>
+    <t>argument names in the image end point and the function must be consistent. They are image_number and id</t>
+  </si>
+  <si>
+    <t>AttributeError: 'Image' object has no attribute 'username'</t>
+  </si>
+  <si>
+    <t>need to change username to user_id</t>
+  </si>
+  <si>
+    <t>Mental Health Surveys</t>
+  </si>
+  <si>
+    <t>Try CRUD operations on surveys</t>
+  </si>
+  <si>
+    <t>Can create, read, update and delete surveys</t>
+  </si>
+  <si>
+    <t>update or delete on table "mental_health_surveys" violates foreign key constraint "survey_questions_mental_health_survey_id_fkey" on table "survey_questions"</t>
+  </si>
+  <si>
+    <t>need to check for any survey questions that are dependent on mental health surveys before deleting a mental health survey</t>
+  </si>
+  <si>
+    <t>Try CRUD operations on the questions</t>
+  </si>
+  <si>
+    <t>Can create, read, update and delete questions</t>
+  </si>
+  <si>
+    <t>missing id and question_text</t>
+  </si>
+  <si>
+    <t>question schema and question model do not match. Need to get rid of id and replace "question_text" with just "text"</t>
+  </si>
+  <si>
+    <t>AttributeError: 'Question' object has no attribute 'update'</t>
+  </si>
+  <si>
+    <t>don't use the .first() method on the question object</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Try CRUD operations on the survey questions</t>
+  </si>
+  <si>
+    <t>Can create, read, update and delete survey questions</t>
+  </si>
+  <si>
+    <t>Cannot see the survey details and question details in the survey question object in json</t>
+  </si>
+  <si>
+    <t>Need to alter the schemas and models so that there is a db.relationship between the question, survey and the survey question</t>
+  </si>
+  <si>
+    <t>Forgot to set the username field</t>
   </si>
 </sst>
 </file>
@@ -573,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E960B6C0-1591-4849-8A39-B1D5B05F6FA6}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,9 +960,7 @@
       <c r="G16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
@@ -853,6 +974,354 @@
         <v>31</v>
       </c>
     </row>
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="8">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="8"/>
+      <c r="F25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F26" s="5"/>
+      <c r="G26" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F31" s="5"/>
+      <c r="G31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>8</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F34" s="5"/>
+      <c r="G34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F37" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G38" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="8">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F41" s="5"/>
+      <c r="G41" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G42" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the manual tests to include CICD pipeline and updated ReadME with trello board screenshots
</commit_message>
<xml_diff>
--- a/docs/manual_tests.xlsx
+++ b/docs/manual_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Coder_Academy\Term_4_Assignment_real\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAEB57C-BE4F-4A27-AA80-0B2F2EC0C55C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6954F047-8D76-4672-B3D2-DA2EA3327BA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9969861-9E08-43B7-8AB0-936C696BF090}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
   <si>
     <t>Feature</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Step</t>
-  </si>
-  <si>
     <t xml:space="preserve">Try to login and see if valid token is returned </t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>Forgot to set the username field</t>
   </si>
   <si>
-    <t>CICD piple</t>
-  </si>
-  <si>
     <t>Run the yml file when pushing to github. This should run automated tests and</t>
   </si>
   <si>
@@ -280,6 +274,51 @@
   </si>
   <si>
     <t>Successfully does automated checks and deployment</t>
+  </si>
+  <si>
+    <t>Pushing to the wrong branch, need to push to main</t>
+  </si>
+  <si>
+    <t>Cannot find discovery file for test suite</t>
+  </si>
+  <si>
+    <t>Need to change workflow to cd into src file so that tests directory may be discovered</t>
+  </si>
+  <si>
+    <t>Blanks in the cicd.yml file cause syntax errors</t>
+  </si>
+  <si>
+    <t>python-dotenv is not in the requirements.txt file</t>
+  </si>
+  <si>
+    <t>Need to pip freeze the virtual environment</t>
+  </si>
+  <si>
+    <t>github actions can find the ssh_key in secrets</t>
+  </si>
+  <si>
+    <t>The EC2 instance needs a private and public key pair</t>
+  </si>
+  <si>
+    <t>db_uri, aws_secret_key and other variables are not set.</t>
+  </si>
+  <si>
+    <t>Use secrets in github to include them</t>
+  </si>
+  <si>
+    <t>github actions complains that wrong python version is being used</t>
+  </si>
+  <si>
+    <t>Change it instead to python3</t>
+  </si>
+  <si>
+    <t>can't install venv in the present working directory</t>
+  </si>
+  <si>
+    <t>Go to a different file</t>
+  </si>
+  <si>
+    <t>CICD pipeline</t>
   </si>
 </sst>
 </file>
@@ -708,25 +747,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E960B6C0-1591-4849-8A39-B1D5B05F6FA6}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="83" customWidth="1"/>
-    <col min="5" max="5" width="53" customWidth="1"/>
-    <col min="6" max="6" width="69.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="114" customWidth="1"/>
+    <col min="3" max="3" width="83" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="5" max="5" width="69.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="114" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -734,75 +772,67 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8">
-        <v>1</v>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
@@ -810,130 +840,114 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="F5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="8">
-        <v>2</v>
-      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="8">
-        <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="8">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="G12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="H12" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" s="8">
-        <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>33</v>
@@ -941,273 +955,247 @@
       <c r="E14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="E15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="8">
-        <v>2</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F17" s="12"/>
+      <c r="G17" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
       <c r="D18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="8">
-        <v>2</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F22" s="12"/>
+      <c r="G22" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="8">
-        <v>1</v>
-      </c>
       <c r="D23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="F23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="8"/>
-      <c r="F25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F26" s="5"/>
-      <c r="G26" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E26" s="5"/>
+      <c r="F26" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F27" s="12"/>
+      <c r="G27" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>7</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="8">
-        <v>1</v>
-      </c>
       <c r="D28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="5" t="s">
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E29" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="5" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E30" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F31" s="5"/>
-      <c r="G31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E31" s="5"/>
+      <c r="F31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="10"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F32" s="12"/>
+      <c r="G32" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>8</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C33" s="8">
-        <v>1</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>62</v>
@@ -1215,44 +1203,40 @@
       <c r="E33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="5"/>
-      <c r="G34" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+      <c r="F34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="10"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F35" s="12"/>
+      <c r="G35" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="8">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>66</v>
@@ -1260,53 +1244,49 @@
       <c r="E36" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="5" t="s">
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E37" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G38" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
-      <c r="C39" s="10"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F39" s="12"/>
+      <c r="G39" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>10</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C40" s="8">
-        <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>73</v>
@@ -1314,64 +1294,132 @@
       <c r="E40" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F41" s="5"/>
-      <c r="G41" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E41" s="5"/>
+      <c r="F41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F42" s="12"/>
+      <c r="G42" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>11</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="8">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C44" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D44" s="5" t="s">
-        <v>80</v>
+      <c r="F44" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E46" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E47" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E48" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E49" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E50" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F51" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added UI tests to excel file
</commit_message>
<xml_diff>
--- a/docs/manual_tests.xlsx
+++ b/docs/manual_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Coder_Academy\Term_4_Assignment_real\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6954F047-8D76-4672-B3D2-DA2EA3327BA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A30F3B-D75E-4FB8-A1D8-07636A0CFE04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9969861-9E08-43B7-8AB0-936C696BF090}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="105">
   <si>
     <t>Feature</t>
   </si>
@@ -319,6 +319,36 @@
   </si>
   <si>
     <t>CICD pipeline</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Can enter in both weekly income sources and weekly expense sources</t>
+  </si>
+  <si>
+    <t>Successfully shows those sources</t>
+  </si>
+  <si>
+    <t>Gender field missing</t>
+  </si>
+  <si>
+    <t>Wrong datatime entered for time</t>
+  </si>
+  <si>
+    <t>'forms.CreateWeeklyExpenseSource object' has no attribute 'income_type'</t>
+  </si>
+  <si>
+    <t>Need to change income to expense</t>
+  </si>
+  <si>
+    <t>The form should automatically check for this.</t>
+  </si>
+  <si>
+    <t>Text box is lift align and looks weird. Should be centered</t>
+  </si>
+  <si>
+    <t>Use in-line style and margin property set to auto</t>
   </si>
 </sst>
 </file>
@@ -747,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E960B6C0-1591-4849-8A39-B1D5B05F6FA6}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1425,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E49" s="5" t="s">
         <v>90</v>
       </c>
@@ -1406,7 +1436,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E50" s="5" t="s">
         <v>92</v>
       </c>
@@ -1417,10 +1447,95 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F51" s="7" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="52" spans="1:7" s="13" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="8">
+        <v>12</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E55" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E56" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E57" s="5"/>
+      <c r="F57" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E58" s="5"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E59" s="5"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E60" s="5"/>
+      <c r="G60" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>